<commit_message>
Uploading backlog of files
</commit_message>
<xml_diff>
--- a/timescale 2.0.xlsx
+++ b/timescale 2.0.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\myfiles\hrh33\dos\FYP Adjustabike\PSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\myfiles\hrh33\dos\FYP Adjustabike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41B0AD1-8ED7-48F2-AED9-6F193BB3056F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278ABE34-A12D-46BD-8DB7-CDA47D5FF512}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="450" xr2:uid="{E5689373-E6E2-464D-A006-4A9C94259F9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$57</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>WP1</t>
   </si>
@@ -187,6 +190,24 @@
   </si>
   <si>
     <t>throughout, build should be documented photographically</t>
+  </si>
+  <si>
+    <t>Research Mechanical Design Synthesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop Design Specification for kit </t>
+  </si>
+  <si>
+    <t>Carry out morphological design for kit</t>
+  </si>
+  <si>
+    <t>Sketch final concept</t>
+  </si>
+  <si>
+    <t>Develop criteria based on concept, specification, and last year's report</t>
+  </si>
+  <si>
+    <t>Decide on weights and scoring system</t>
   </si>
 </sst>
 </file>
@@ -577,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3FCC02-3CF7-4DB2-9D2B-903EC04A86FE}">
-  <dimension ref="A2:C51"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,495 +610,538 @@
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>43</v>
+      <c r="A2" s="5">
+        <v>43796</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43796</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="6"/>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>43796</v>
       </c>
-      <c r="B3" s="1">
-        <v>43796</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="C4" s="2" t="s">
-        <v>0</v>
+      <c r="B4" s="1">
+        <v>43864</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>43796</v>
+        <v>43801</v>
       </c>
       <c r="B5" s="1">
-        <v>43864</v>
+        <v>43866</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>43801</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43866</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
+      <c r="A6" s="5"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>43806</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43867</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
+      <c r="A7" s="5"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>43856</v>
-      </c>
-      <c r="B8" s="1">
-        <v>43871</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
+      <c r="A8" s="5"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>43859</v>
-      </c>
-      <c r="B9" s="1">
-        <v>43874</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
+      <c r="A9" s="5"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>43860</v>
-      </c>
-      <c r="B10" s="1">
-        <v>43875</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
+      <c r="A10" s="5"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
+      <c r="A11" s="5"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>43864</v>
+        <v>43806</v>
       </c>
       <c r="B12" s="1">
-        <v>43878</v>
+        <v>43867</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>43864</v>
+        <v>43856</v>
       </c>
       <c r="B13" s="1">
-        <v>43879</v>
+        <v>43871</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>43867</v>
+        <v>43859</v>
       </c>
       <c r="B14" s="1">
-        <v>43879</v>
+        <v>43874</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>43868</v>
+        <v>43860</v>
       </c>
       <c r="B15" s="1">
-        <v>43880</v>
+        <v>43875</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>43871</v>
-      </c>
-      <c r="B16" s="1">
-        <v>43881</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
+      <c r="A16" s="6"/>
+      <c r="C16" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>43873</v>
+        <v>43864</v>
       </c>
       <c r="B17" s="1">
-        <v>43881</v>
+        <v>43878</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="A18" s="5">
+        <v>43864</v>
+      </c>
       <c r="B18" s="1">
-        <v>43882</v>
+        <v>43879</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>43880</v>
+        <v>43867</v>
       </c>
       <c r="B19" s="1">
-        <v>43885</v>
+        <v>43879</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>43887</v>
+        <v>43868</v>
       </c>
       <c r="B20" s="1">
-        <v>43887</v>
+        <v>43880</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="C21" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="C22" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>43876</v>
-      </c>
+      <c r="A21" s="5">
+        <v>43871</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43881</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>43873</v>
+      </c>
+      <c r="B22" s="1">
+        <v>43881</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
       <c r="B23" s="1">
-        <v>43883</v>
+        <v>43882</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>43888</v>
+        <v>43880</v>
       </c>
       <c r="B24" s="1">
-        <v>43888</v>
+        <v>43885</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>43888</v>
+        <v>43887</v>
       </c>
       <c r="B25" s="1">
-        <v>43889</v>
+        <v>43887</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="6"/>
+      <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="C27" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>43876</v>
       </c>
-      <c r="B26" s="1">
-        <v>43882</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="1">
-        <v>43862</v>
-      </c>
-      <c r="C27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>43895</v>
-      </c>
       <c r="B28" s="1">
-        <v>43894</v>
+        <v>43883</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>43893</v>
+        <v>43888</v>
       </c>
       <c r="B29" s="1">
-        <v>43896</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>40</v>
+        <v>43888</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
+        <v>43888</v>
+      </c>
+      <c r="B30" s="1">
+        <v>43889</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>43876</v>
+      </c>
+      <c r="B31" s="1">
+        <v>43882</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="1">
+        <v>43862</v>
+      </c>
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>43895</v>
+      </c>
+      <c r="B33" s="1">
+        <v>43894</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>43893</v>
+      </c>
+      <c r="B34" s="1">
+        <v>43896</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
         <v>43536</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B35" s="1">
         <v>43536</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C35" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="C31" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>43796</v>
-      </c>
-      <c r="B32" s="1">
-        <v>43864</v>
-      </c>
-      <c r="C32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="1">
-        <v>43864</v>
-      </c>
-      <c r="C33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="1">
-        <v>43796</v>
-      </c>
-      <c r="C34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="1">
-        <v>43866</v>
-      </c>
-      <c r="C35" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="1">
-        <v>43902</v>
-      </c>
-      <c r="C36" t="s">
-        <v>23</v>
+      <c r="C36" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="A37" s="5">
+        <v>43796</v>
+      </c>
       <c r="B37" s="1">
-        <v>43909</v>
+        <v>43864</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="1">
-        <v>43909</v>
+        <v>43864</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
-      <c r="C39" s="2" t="s">
-        <v>25</v>
+      <c r="B39" s="1">
+        <v>43796</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>43918</v>
-      </c>
+      <c r="A40" s="6"/>
       <c r="B40" s="1">
-        <v>43920</v>
+        <v>43866</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="1">
-        <v>43922</v>
+        <v>43902</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="1">
-        <v>43923</v>
+        <v>43909</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="1">
-        <v>43924</v>
+        <v>43909</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="1">
-        <v>43927</v>
-      </c>
-      <c r="C44" t="s">
-        <v>29</v>
+      <c r="C44" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="A45" s="5">
+        <v>43918</v>
+      </c>
       <c r="B45" s="1">
-        <v>43928</v>
+        <v>43920</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="1">
-        <v>43934</v>
+        <v>43922</v>
       </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="1">
-        <v>43941</v>
+        <v>43923</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="1">
+        <v>43924</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="1">
+        <v>43927</v>
+      </c>
+      <c r="C49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="1">
+        <v>43928</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="1">
+        <v>43934</v>
+      </c>
+      <c r="C51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="1">
+        <v>43941</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+      <c r="B53" s="1">
         <v>43914</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C53" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
         <v>43950</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B54" s="1">
         <v>43950</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
         <v>43962</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B55" s="1">
         <v>43962</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
         <v>43976</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B56" s="1">
         <v>43976</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C56" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C57" xr:uid="{D2D70695-6DC5-454A-B209-C12D1411A371}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated design synthesis 05/02
</commit_message>
<xml_diff>
--- a/timescale 2.0.xlsx
+++ b/timescale 2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\myfiles\hrh33\dos\FYP Adjustabike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278ABE34-A12D-46BD-8DB7-CDA47D5FF512}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F3332E-2D1A-489A-A27E-2F7CF1317A24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="450" xr2:uid="{E5689373-E6E2-464D-A006-4A9C94259F9D}"/>
   </bookViews>
@@ -601,7 +601,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,42 +662,54 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>43866</v>
+      </c>
       <c r="C6" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>43867</v>
+      </c>
       <c r="C7" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>43867</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1">
+        <v>43867</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1">
+        <v>43867</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1">
+        <v>43867</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>57</v>
       </c>
@@ -707,7 +719,7 @@
         <v>43806</v>
       </c>
       <c r="B12" s="1">
-        <v>43867</v>
+        <v>43868</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
forgot to save WP2 update
</commit_message>
<xml_diff>
--- a/timescale 2.0.xlsx
+++ b/timescale 2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\myfiles\hrh33\dos\FYP Adjustabike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F3332E-2D1A-489A-A27E-2F7CF1317A24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFECB34-9146-4C4D-B86A-85EFC3CBA548}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="450" xr2:uid="{E5689373-E6E2-464D-A006-4A9C94259F9D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>WP1</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Decide on weights and scoring system</t>
+  </si>
+  <si>
+    <t>Develop criteria for geometries/ assemblies</t>
   </si>
 </sst>
 </file>
@@ -598,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3FCC02-3CF7-4DB2-9D2B-903EC04A86FE}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,130 +772,128 @@
         <v>43864</v>
       </c>
       <c r="B17" s="1">
-        <v>43878</v>
+        <v>43875</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>43864</v>
-      </c>
+      <c r="A18" s="5"/>
       <c r="B18" s="1">
-        <v>43879</v>
+        <v>43878</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>43867</v>
+        <v>43864</v>
       </c>
       <c r="B19" s="1">
         <v>43879</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>43868</v>
+        <v>43867</v>
       </c>
       <c r="B20" s="1">
-        <v>43880</v>
+        <v>43879</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>43871</v>
+        <v>43868</v>
       </c>
       <c r="B21" s="1">
-        <v>43881</v>
+        <v>43880</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>43873</v>
+        <v>43871</v>
       </c>
       <c r="B22" s="1">
         <v>43881</v>
       </c>
       <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>43873</v>
+      </c>
+      <c r="B23" s="1">
+        <v>43881</v>
+      </c>
+      <c r="C23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="1">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="1">
         <v>43882</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>43880</v>
-      </c>
-      <c r="B24" s="1">
-        <v>43885</v>
-      </c>
-      <c r="C24" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
+        <v>43880</v>
+      </c>
+      <c r="B25" s="1">
+        <v>43885</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>43887</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B26" s="1">
         <v>43887</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="C26" s="2" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="C27" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="C27" s="7" t="s">
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="C28" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>43876</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B29" s="1">
         <v>43883</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>43888</v>
-      </c>
-      <c r="B29" s="1">
-        <v>43888</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -900,125 +901,127 @@
         <v>43888</v>
       </c>
       <c r="B30" s="1">
-        <v>43889</v>
+        <v>43888</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
+        <v>43888</v>
+      </c>
+      <c r="B31" s="1">
+        <v>43889</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>43876</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B32" s="1">
         <v>43882</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="1">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="1">
         <v>43862</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>43895</v>
-      </c>
-      <c r="B33" s="1">
-        <v>43894</v>
-      </c>
-      <c r="C33" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>43893</v>
+        <v>43895</v>
       </c>
       <c r="B34" s="1">
-        <v>43896</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>40</v>
+        <v>43894</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
+        <v>43893</v>
+      </c>
+      <c r="B35" s="1">
+        <v>43896</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
         <v>43536</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B36" s="1">
         <v>43536</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="C36" s="2" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="C37" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
         <v>43796</v>
       </c>
-      <c r="B37" s="1">
-        <v>43864</v>
-      </c>
-      <c r="C37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
       <c r="B38" s="1">
         <v>43864</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="1">
-        <v>43796</v>
+        <v>43864</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="1">
-        <v>43866</v>
+        <v>43796</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="1">
-        <v>43902</v>
+        <v>43866</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="1">
-        <v>43909</v>
+        <v>43902</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,133 +1030,142 @@
         <v>43909</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="C44" s="2" t="s">
+      <c r="B44" s="1">
+        <v>43909</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="C45" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
         <v>43918</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B46" s="1">
         <v>43920</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="1">
-        <v>43922</v>
-      </c>
-      <c r="C46" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="C47" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="1">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="1">
-        <v>43927</v>
+        <v>43924</v>
       </c>
       <c r="C49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="1">
-        <v>43928</v>
+        <v>43927</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="1">
-        <v>43934</v>
+        <v>43928</v>
       </c>
       <c r="C51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="1">
-        <v>43941</v>
+        <v>43934</v>
       </c>
       <c r="C52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="1">
+        <v>43941</v>
+      </c>
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="1">
         <v>43914</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
-        <v>43950</v>
-      </c>
-      <c r="B54" s="1">
-        <v>43950</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>43962</v>
+        <v>43950</v>
       </c>
       <c r="B55" s="1">
-        <v>43962</v>
+        <v>43950</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
+        <v>43962</v>
+      </c>
+      <c r="B56" s="1">
+        <v>43962</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
         <v>43976</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B57" s="1">
         <v>43976</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C57" xr:uid="{D2D70695-6DC5-454A-B209-C12D1411A371}"/>
+  <autoFilter ref="A1:C58" xr:uid="{D2D70695-6DC5-454A-B209-C12D1411A371}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>